<commit_message>
kavenegar message send but multiple error
</commit_message>
<xml_diff>
--- a/a.xlsx
+++ b/a.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Python\Desktop\project\first-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478FB5CD-D5C1-4656-9C6B-37AEA528C684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A33292-5621-4EC5-9EC0-10353CB94922}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,10 +441,13 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -471,7 +474,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1564454</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -488,7 +491,7 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>1564454</v>
+        <v>9120044824</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>

</xml_diff>